<commit_message>
Fix #22457 - [Feature] Search exports update
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/client/en/ExportClientSurvey.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/client/en/ExportClientSurvey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Client" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Client!$B$3:$G$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Survey!$B$3:$H$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Survey!$B$3:$I$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
@@ -84,7 +84,7 @@
     <t xml:space="preserve">entity|cm:name</t>
   </si>
   <si>
-    <t xml:space="preserve">bcpg:variantIds</t>
+    <t xml:space="preserve">entity|bcpg:code</t>
   </si>
   <si>
     <t xml:space="preserve">survey:slQuestion</t>
@@ -99,7 +99,7 @@
     <t xml:space="preserve">Entity name</t>
   </si>
   <si>
-    <t xml:space="preserve">Variants</t>
+    <t xml:space="preserve">beCPG code</t>
   </si>
   <si>
     <t xml:space="preserve">Question</t>
@@ -364,11 +364,11 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.98"/>
@@ -452,7 +452,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -461,9 +461,11 @@
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="4" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="4" width="25.98"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="4" min="3" style="4" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="4" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="4" width="13.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="996" min="9" style="4" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="55.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="34.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="36.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="997" min="10" style="4" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -479,6 +481,7 @@
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="23.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -494,18 +497,20 @@
         <v>18</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -518,6 +523,7 @@
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
     </row>
     <row r="3" s="10" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
@@ -533,18 +539,20 @@
         <v>23</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="ALI3" s="0"/>
       <c r="ALJ3" s="0"/>
       <c r="ALK3" s="0"/>
       <c r="ALL3" s="0"/>
@@ -574,7 +582,7 @@
       <c r="AMJ3" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:H3"/>
+  <autoFilter ref="B3:I3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>